<commit_message>
Excel de recogida de datos definitivo
</commit_message>
<xml_diff>
--- a/MUESTREOS.xlsx
+++ b/MUESTREOS.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>coor_x</t>
   </si>
@@ -41,42 +42,21 @@
     <t>fecha</t>
   </si>
   <si>
-    <t>estación</t>
-  </si>
-  <si>
     <t>sp.</t>
   </si>
   <si>
-    <t>perímetro_tronco</t>
-  </si>
-  <si>
     <t>dist_vert</t>
   </si>
   <si>
-    <t>pendiente</t>
-  </si>
-  <si>
-    <t>num_arboles_10_m</t>
-  </si>
-  <si>
-    <t>alt_primera_rama</t>
-  </si>
-  <si>
     <t>num_piñas_roidas</t>
   </si>
   <si>
-    <t>altitud_media</t>
-  </si>
-  <si>
     <t>nivel_sotobos</t>
   </si>
   <si>
     <t>obs</t>
   </si>
   <si>
-    <t>reposicion</t>
-  </si>
-  <si>
     <t>fecha_2da_visita</t>
   </si>
   <si>
@@ -84,13 +64,121 @@
   </si>
   <si>
     <t>obs_rep</t>
+  </si>
+  <si>
+    <t>estac</t>
+  </si>
+  <si>
+    <t>perím_tronco</t>
+  </si>
+  <si>
+    <t>pend</t>
+  </si>
+  <si>
+    <t>num_arbol_10_m</t>
+  </si>
+  <si>
+    <t>alt_1a_rama</t>
+  </si>
+  <si>
+    <t>reposic</t>
+  </si>
+  <si>
+    <t>Ph_01</t>
+  </si>
+  <si>
+    <t>Cumbres Verdes</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Ph</t>
+  </si>
+  <si>
+    <t>Lad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEYENDA </t>
+  </si>
+  <si>
+    <t>Significado</t>
+  </si>
+  <si>
+    <t>Código del pino (Ph_01: Pinus halepensis número 1, etc.)</t>
+  </si>
+  <si>
+    <t>Localización (Nombre parcela)</t>
+  </si>
+  <si>
+    <t>Fecha de toma de datos</t>
+  </si>
+  <si>
+    <t>coor_x e y</t>
+  </si>
+  <si>
+    <t>Coordenadas del pino</t>
+  </si>
+  <si>
+    <t>Estación del año</t>
+  </si>
+  <si>
+    <t>Especie de pino</t>
+  </si>
+  <si>
+    <t>Perímetro del tronco (1,3m)</t>
+  </si>
+  <si>
+    <t>Distancia vertical</t>
+  </si>
+  <si>
+    <t>Pendiente (llano/ladera)</t>
+  </si>
+  <si>
+    <t>Nº de árboles en 10 metros</t>
+  </si>
+  <si>
+    <t>Altura de la 1ª rama de 5 cm diámetro</t>
+  </si>
+  <si>
+    <t>Nº piñas roídas</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Reposición (SÍ/NO)</t>
+  </si>
+  <si>
+    <t>Fecha de la 2ª visita</t>
+  </si>
+  <si>
+    <t>Nº de piñas roídas en la 2ª visita</t>
+  </si>
+  <si>
+    <t>Observaciones de la reposición</t>
+  </si>
+  <si>
+    <t>Nivel de sotobosque</t>
+  </si>
+  <si>
+    <t>Código columna</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>SÍ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +186,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,8 +221,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,96 +509,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
     <col min="7" max="7" width="4.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44874</v>
+      </c>
+      <c r="D2">
+        <v>450404</v>
+      </c>
+      <c r="E2">
+        <v>4106870</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>151</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <v>261</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>44913</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>